<commit_message>
added critiques & history page
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TODO" sheetId="1" r:id="rId1"/>
+    <sheet name="History &amp; Critiques" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -50,12 +49,24 @@
   <si>
     <t>fine-tune following camera, resetting</t>
   </si>
+  <si>
+    <t>History &amp; Critiques</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Critiques</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,13 +89,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -117,15 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -146,6 +167,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,7 +191,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
@@ -174,21 +224,7 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -196,21 +232,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B36" totalsRowShown="0" headerRowDxfId="7" dataDxfId="2" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B36" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A2:B36"/>
   <tableColumns count="2">
-    <tableColumn id="2" name="Programming" dataDxfId="4"/>
-    <tableColumn id="8" name="Art" dataDxfId="3"/>
+    <tableColumn id="2" name="Programming" dataDxfId="5"/>
+    <tableColumn id="8" name="Art" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C2:C36" totalsRowShown="0" dataDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C2:C36" totalsRowShown="0" dataDxfId="2" headerRowBorderDxfId="3" tableBorderDxfId="1">
   <autoFilter ref="C2:C36"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Combined" dataDxfId="1"/>
+    <tableColumn id="1" name="Combined" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -503,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -515,11 +551,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -528,193 +564,193 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="30">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" ht="30">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -731,24 +767,672 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="26.25">
+      <c r="A1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="6"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="6"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="6"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="6"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="6"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="6"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="6"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="6"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="6"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="6"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="6"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="6"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="6"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="6"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="6"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="6"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="6"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="6"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="6"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="6"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="6"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="6"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="6"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="6"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="6"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="6"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="6"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="6"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="6"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="6"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="6"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="6"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="6"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="6"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="6"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="75">
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added links to version builds
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -106,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +142,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -185,10 +192,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -220,17 +231,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -817,7 +832,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -827,624 +842,623 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="60" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:14" ht="61.5" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="6"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="6"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="6"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="6"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="6"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="6"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="6"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="6"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="6"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="6"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="6"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="6"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="6"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="6"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="6"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="6"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="6"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="6"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="6"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="6"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="6"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="6"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="6"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="6"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="6"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="6"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="6"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="6"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="6"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="6"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="6"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="6"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="6"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="6"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1461,37 +1475,42 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new build v0.3, updated todo
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -104,12 +104,20 @@
   <si>
     <t>Need to know exactly how camera will operate</t>
   </si>
+  <si>
+    <t>Better camera following
+Sped up time a bit.
+Fixed some reset problems.</t>
+  </si>
+  <si>
+    <t>v 0.3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +160,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -202,7 +216,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -248,6 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -607,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -676,7 +693,7 @@
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5"/>
@@ -839,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -926,9 +943,13 @@
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="6"/>
-      <c r="B5" s="13"/>
+    <row r="5" spans="1:14" ht="51.75" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -1438,36 +1459,35 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1484,41 +1504,43 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
version 4, updated todo.xlsx, added KEYS.txt, camera now uses zoom in/out preset positions to interpolate between with gui button (top-left)
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -111,6 +111,13 @@
   </si>
   <si>
     <t>v 0.3</t>
+  </si>
+  <si>
+    <t>v 0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera now interpolates between 2 positions for zoom in/out
+</t>
   </si>
 </sst>
 </file>
@@ -251,6 +258,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,9 +272,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -636,11 +643,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -693,7 +700,7 @@
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5"/>
@@ -857,7 +864,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -867,627 +874,632 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:14" ht="60" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:14" ht="61.5" customHeight="1">
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:14" ht="51.75" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="6"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
+      <c r="A6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="6"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="6"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="6"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="6"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="6"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="6"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="6"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="6"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="6"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="6"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="6"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="6"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="6"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="6"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="6"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="6"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="6"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="6"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="6"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="6"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="6"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="6"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="6"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="6"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="6"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="6"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="6"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="6"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="6"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="6"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="6"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="6"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1504,43 +1516,43 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="A4" r:id="rId2"/>
     <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated todo.xlsx with v0.5
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -120,13 +120,12 @@
 </t>
   </si>
   <si>
-    <t>To have two main cameras that quickly zoom between each other; adding perspective to the 3D side scroll style. One camera display the entire level, the other centering on the character; adding some drag to the camera would feel more natural.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Camera movement is very smooth. Practice level has floor, backing, and a ceiling, its nice to know what your limits are in the beginning of a game, and to exceed them over time. The character motion was at good speed; I think the landing should be a harder drop, like the character "spacks" the ground, maybe a short skid. ( I actually, flung myelf into the ceiling and it was awesome, it just bounced off straight to the ground.) I also enjoy the movement on the pivot point and the weight, they seem to be smoother as well. and the see-saw to triangle ratio is more aesthetically pleasing.</t>
+    <t>v 0.5</t>
+  </si>
+  <si>
+    <t>Added ceiling and back wall
+added rough main menu, transition with play button
+start level with camera zoomed out on entire level, wait a bit, then zoom in on see-saw</t>
   </si>
 </sst>
 </file>
@@ -870,10 +869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:M5"/>
+      <selection activeCell="B9" sqref="B9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -952,9 +951,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="14" t="s">
-        <v>24</v>
-      </c>
+      <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
@@ -980,7 +977,7 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:14" ht="126.75" customHeight="1">
+    <row r="6" spans="1:14">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -992,18 +989,20 @@
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="14"/>
+    <row r="7" spans="1:14" ht="45.75" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -1481,42 +1480,38 @@
       <c r="L38" s="14"/>
       <c r="M38" s="14"/>
     </row>
-    <row r="39" spans="1:13">
-      <c r="M39" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1533,44 +1528,44 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="A4" r:id="rId2"/>
     <hyperlink ref="A5" r:id="rId3"/>
     <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merged with mike's comments
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -126,6 +126,12 @@
     <t>Added ceiling and back wall
 added rough main menu, transition with play button
 start level with camera zoomed out on entire level, wait a bit, then zoom in on see-saw</t>
+  </si>
+  <si>
+    <t>Camera movement is very smooth. Practice level has floor, backing, and a ceiling, its nice to know what your limits are in the beginning of a game, and to exceed them over time. The character motion was at good speed; I think the landing should be a harder drop, like the character "spacks" the ground, maybe a short skid. ( I actually, flung myelf into the ceiling and it was awesome, it just bounced off straight to the ground.) I also enjoy the movement on the pivot point and the weight, they seem to be smoother as well. and the see-saw to triangle ratio is more aesthetically pleasing.</t>
+  </si>
+  <si>
+    <t>To have two main cameras that quickly zoom between each other; adding perspective to the 3D side scroll style. One camera display the entire level, the other centering on the character; adding some drag to the camera would feel more natural.</t>
   </si>
 </sst>
 </file>
@@ -872,7 +878,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:G9"/>
+      <selection activeCell="H5" sqref="H5:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -951,7 +957,9 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="H4" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
@@ -996,7 +1004,7 @@
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="1:14" ht="45.75" customHeight="1">
+    <row r="7" spans="1:14" ht="127.5" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
@@ -1008,7 +1016,9 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="H7" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -1482,36 +1492,35 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1528,35 +1537,36 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
version 0.8, updated todo.xlsx
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -160,6 +160,14 @@
   </si>
   <si>
     <t>Jump pad now uses player's velocity to determine force player is propelled away with</t>
+  </si>
+  <si>
+    <t>v 0.8</t>
+  </si>
+  <si>
+    <t>Jump pads more realistic, feel better
+brought zoomed in cam out a bit,
+Cam now follows the player's y movement</t>
   </si>
 </sst>
 </file>
@@ -931,7 +939,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1116,9 +1124,13 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="6"/>
-      <c r="B10" s="16"/>
+    <row r="10" spans="1:14" ht="45" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -1553,36 +1565,35 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1599,35 +1610,36 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -1637,8 +1649,9 @@
     <hyperlink ref="A7" r:id="rId5"/>
     <hyperlink ref="A8" r:id="rId6"/>
     <hyperlink ref="A9" r:id="rId7"/>
+    <hyperlink ref="A10" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added version 0.9, updated todo.xlsx
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -168,6 +168,16 @@
     <t>Jump pads more realistic, feel better
 brought zoomed in cam out a bit,
 Cam now follows the player's y movement</t>
+  </si>
+  <si>
+    <t>v 0.9</t>
+  </si>
+  <si>
+    <t>Added a second level to test transitioning
+Added defeat scene
+Added code to die when spikes are hit
+Added delay for reset after dying
+Added lives &amp; health (in code only)</t>
   </si>
 </sst>
 </file>
@@ -939,7 +949,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1143,9 +1153,13 @@
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="6"/>
-      <c r="B11" s="16"/>
+    <row r="11" spans="1:14" ht="81" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1565,35 +1579,36 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1610,36 +1625,35 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -1650,8 +1664,9 @@
     <hyperlink ref="A8" r:id="rId6"/>
     <hyperlink ref="A9" r:id="rId7"/>
     <hyperlink ref="A10" r:id="rId8"/>
+    <hyperlink ref="A11" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated version 0.9 (to 0.9.1), updated link in todo.xlsx
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -170,14 +170,14 @@
 Cam now follows the player's y movement</t>
   </si>
   <si>
-    <t>v 0.9</t>
-  </si>
-  <si>
     <t>Added a second level to test transitioning
 Added defeat scene
 Added code to die when spikes are hit
 Added delay for reset after dying
 Added lives &amp; health (in code only)</t>
+  </si>
+  <si>
+    <t>v 0.9.1</t>
   </si>
 </sst>
 </file>
@@ -949,7 +949,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1155,10 +1155,10 @@
     </row>
     <row r="11" spans="1:14" ht="81" customHeight="1">
       <c r="A11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -1579,36 +1579,35 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1625,35 +1624,36 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -1664,7 +1664,7 @@
     <hyperlink ref="A8" r:id="rId6"/>
     <hyperlink ref="A9" r:id="rId7"/>
     <hyperlink ref="A10" r:id="rId8"/>
-    <hyperlink ref="A11" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId9" display="v 0.9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>

</xml_diff>

<commit_message>
added critique to version 9.1 of see-saw tests
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>v 0.9.1</t>
+  </si>
+  <si>
+    <t>The flow is getting to a really good point! And the new camera adjustment adds a lot more to it. I think the player should be able to bring the weight a little bit farther down closer to the see-saw; in order to create a short hop over objects. I like the limits side-to-side. The bouce amount from the jump pads can have more spring to them, propelling the character farther. The level change adds an extra encentive to completing the level, and allows more personal gain, nice touch.</t>
   </si>
 </sst>
 </file>
@@ -949,7 +952,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H12" sqref="H12:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1115,7 +1118,7 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" ht="33.75" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>35</v>
       </c>
@@ -1165,7 +1168,9 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+      <c r="H11" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
@@ -1579,35 +1584,36 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1624,36 +1630,35 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
version 0.10, updated todo.xlsx
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -181,6 +181,17 @@
   </si>
   <si>
     <t>The flow is getting to a really good point! And the new camera adjustment adds a lot more to it. I think the player should be able to bring the weight a little bit farther down closer to the see-saw; in order to create a short hop over objects. I like the limits side-to-side. The bouce amount from the jump pads can have more spring to them, propelling the character farther. The level change adds an extra encentive to completing the level, and allows more personal gain, nice touch.</t>
+  </si>
+  <si>
+    <t>v 0.10</t>
+  </si>
+  <si>
+    <t>Rearranged levels 1 &amp; 2 to be like concepts
+Tweaked bounce pads to be more responsive
+Added text for death
+Character stops movement when hitting spikes
+Bug fixes for lives counter, resetting correctly…
+Added prefabs for spiked walls, left facing, right facing, both sides</t>
   </si>
 </sst>
 </file>
@@ -951,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:M12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1156,7 +1167,7 @@
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:14" ht="81" customHeight="1">
+    <row r="11" spans="1:14" ht="112.5" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>40</v>
       </c>
@@ -1177,9 +1188,13 @@
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
     </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="6"/>
-      <c r="B12" s="16"/>
+    <row r="12" spans="1:14" ht="93" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1584,36 +1599,35 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1630,35 +1644,36 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -1670,8 +1685,9 @@
     <hyperlink ref="A9" r:id="rId7"/>
     <hyperlink ref="A10" r:id="rId8"/>
     <hyperlink ref="A11" r:id="rId9" display="v 0.9"/>
+    <hyperlink ref="A12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
forgot a change for v0.10
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -191,7 +191,8 @@
 Added text for death
 Character stops movement when hitting spikes
 Bug fixes for lives counter, resetting correctly…
-Added prefabs for spiked walls, left facing, right facing, both sides</t>
+Added prefabs for spiked walls, left facing, right facing, both sides
+increased range for weight movement</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1189,7 @@
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
     </row>
-    <row r="12" spans="1:14" ht="93" customHeight="1">
+    <row r="12" spans="1:14" ht="105.75" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
@@ -1599,35 +1600,36 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1644,36 +1646,35 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
version 0.11, updated todo.xlsx
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>button &amp; menu interaction</t>
+  </si>
+  <si>
+    <t>Determine how we want resetting to work for sure…do we move see saw, subtract health, etc. Flow chart would be good: player comes to rest…what happens after this???</t>
+  </si>
+  <si>
+    <t>v 0.11</t>
+  </si>
+  <si>
+    <t>See-saw now moves to the last place your character stopped if you have enough health
+Keeping track of health and displaying
+Reset health when lives get decremented
+Increased zoomed out camera distance slightly</t>
   </si>
 </sst>
 </file>
@@ -358,6 +370,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,15 +390,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -737,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -750,11 +762,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5">
@@ -772,13 +784,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -821,7 +833,7 @@
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="11"/>
@@ -852,10 +864,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="60">
       <c r="A12" s="11"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11"/>
@@ -994,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:G13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1005,662 +1019,665 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
     </row>
     <row r="3" spans="1:14" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="1:14" ht="61.5" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:14" ht="51.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" spans="1:14" ht="127.5" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" spans="1:14" ht="30.75" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
     </row>
     <row r="9" spans="1:14" ht="33.75" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" spans="1:14" ht="45" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
     </row>
     <row r="11" spans="1:14" ht="112.5" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
     </row>
     <row r="12" spans="1:14" ht="105.75" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="4"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+    </row>
+    <row r="13" spans="1:14" ht="58.5" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="4"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="4"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="4"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="4"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="4"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="4"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="4"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="4"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="4"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="4"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="4"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="4"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="4"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="4"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="4"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="4"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="4"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="4"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="4"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="4"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1677,35 +1694,36 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -1718,8 +1736,9 @@
     <hyperlink ref="A10" r:id="rId8"/>
     <hyperlink ref="A11" r:id="rId9" display="v 0.9"/>
     <hyperlink ref="A12" r:id="rId10"/>
+    <hyperlink ref="A13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to design & todo.xlsx
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -220,6 +220,9 @@
 Keeping track of health and displaying
 Reset health when lives get decremented
 Increased zoomed out camera distance slightly</t>
+  </si>
+  <si>
+    <t>setup rope prefab (character able to move up &amp; down and jump on/off)</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -390,6 +393,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -749,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -847,7 +853,7 @@
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="11"/>
@@ -856,7 +862,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="11"/>
@@ -865,7 +871,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="60">
-      <c r="A12" s="11"/>
+      <c r="A12" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="B12" s="9"/>
       <c r="C12" s="11" t="s">
         <v>49</v>
@@ -1008,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:G15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1649,35 +1657,36 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1694,36 +1703,35 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
version 0.13 - fix for chain not being able to always be grabbed, made grab window to be less, allowing for more realistic positioning on the rope
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -235,6 +235,25 @@
   </si>
   <si>
     <t>setup rope prefab (character able to jump on/off)</t>
+  </si>
+  <si>
+    <t>Allow changing the current level to any level for testing purposes</t>
+  </si>
+  <si>
+    <t>v 0.12</t>
+  </si>
+  <si>
+    <t>Chain rope now can be grabbed correctly no matter what position/orientation it has
+Area to grab onto rope decreased, making where the player is in relation to the rope more realistic looking.</t>
+  </si>
+  <si>
+    <t>v 0.13</t>
+  </si>
+  <si>
+    <t>Added chain rope prefab, player can grab onto it and let go by pressing/releasing 'J'</t>
+  </si>
+  <si>
+    <t>Add dynamic creation of chain rope, being able to add various amount of links through an editor property</t>
   </si>
 </sst>
 </file>
@@ -348,7 +367,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -381,6 +400,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,26 +433,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -773,7 +795,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -785,11 +807,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5">
@@ -807,13 +829,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -821,13 +843,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -835,99 +857,103 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:5" ht="150">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="18" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" ht="45">
+      <c r="A17" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="9"/>
@@ -1042,7 +1068,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:G17"/>
+      <selection activeCell="B16" sqref="B16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1052,666 +1078,673 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:14" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
     </row>
     <row r="4" spans="1:14" ht="61.5" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
     </row>
     <row r="5" spans="1:14" ht="51.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
     </row>
     <row r="7" spans="1:14" ht="127.5" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
     </row>
     <row r="8" spans="1:14" ht="30.75" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
     </row>
     <row r="9" spans="1:14" ht="33.75" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
     </row>
     <row r="10" spans="1:14" ht="45" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
     </row>
     <row r="11" spans="1:14" ht="112.5" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
     </row>
     <row r="12" spans="1:14" ht="105.75" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
     </row>
     <row r="13" spans="1:14" ht="58.5" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="4"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" spans="1:14" ht="16.5" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="4"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
+      <c r="A15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="4"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="4"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="4"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="4"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="4"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="4"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="4"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="4"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="4"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="4"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="4"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="4"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="4"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="4"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="4"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="4"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="4"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="4"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1728,35 +1761,36 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -1770,8 +1804,10 @@
     <hyperlink ref="A11" r:id="rId9" display="v 0.9"/>
     <hyperlink ref="A12" r:id="rId10"/>
     <hyperlink ref="A13" r:id="rId11"/>
+    <hyperlink ref="A15" r:id="rId12" display="v 0.12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added version 0.14 - up/down rope movement, updated todo.xlsx
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15390" windowHeight="8565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -254,6 +254,17 @@
   </si>
   <si>
     <t>Add dynamic creation of chain rope, being able to add various amount of links through an editor property</t>
+  </si>
+  <si>
+    <t>Moving up/down rope - do they automatically stop moving when they get to the bottom, or does that cause them to let go??</t>
+  </si>
+  <si>
+    <t>v0.14</t>
+  </si>
+  <si>
+    <t>Added rough up/down movement for rope
+Added rope reset
+Raised the roof!</t>
   </si>
 </sst>
 </file>
@@ -794,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -872,12 +883,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5" ht="45">
       <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="17" t="s">
@@ -928,7 +941,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="12"/>
@@ -1067,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:G16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1369,9 +1382,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="4"/>
-      <c r="B16" s="20"/>
+    <row r="16" spans="1:14" ht="45.75" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -1806,8 +1823,9 @@
     <hyperlink ref="A13" r:id="rId11"/>
     <hyperlink ref="A15" r:id="rId12" display="v 0.12"/>
     <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A16" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved some currently unused concepts to Misc folder, added levels 1-4, practice level, water, checkpoints, & more
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15390" windowHeight="8565"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15390" windowHeight="8565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -274,6 +274,21 @@
   </si>
   <si>
     <t>determine scale of everything so, figure out a standard for block sizes</t>
+  </si>
+  <si>
+    <t>SCALE IS 6.5</t>
+  </si>
+  <si>
+    <t>v0.16</t>
+  </si>
+  <si>
+    <t>Previous level one is now "practice" level
+Levels 1-4 are done similar to concept images
+Addition of checkpoint prefab
+Addition of water prefab
+Brought zoomed-in cam back a bit
+Added boost force when "J" is pressed
+Many minor changes to code structure &amp; cleanup</t>
   </si>
 </sst>
 </file>
@@ -393,7 +408,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -448,6 +463,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -823,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -836,11 +854,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5">
@@ -889,7 +907,9 @@
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:5" ht="30">
@@ -987,7 +1007,7 @@
       <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" ht="30">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B18" s="9"/>
@@ -1100,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1111,649 +1131,653 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:14" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="4" spans="1:14" ht="61.5" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:14" ht="51.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:14" ht="127.5" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
     </row>
     <row r="8" spans="1:14" ht="30.75" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:14" ht="33.75" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
     </row>
     <row r="10" spans="1:14" ht="45" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
     </row>
     <row r="11" spans="1:14" ht="112.5" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
     </row>
     <row r="12" spans="1:14" ht="105.75" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
     </row>
     <row r="13" spans="1:14" ht="58.5" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" spans="1:14" ht="16.5" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
     </row>
     <row r="16" spans="1:14" ht="45.75" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="4"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+    </row>
+    <row r="18" spans="1:13" ht="105" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="4"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="4"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="4"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="4"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="4"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="4"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="4"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="4"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="4"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="4"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="4"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="4"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="4"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="4"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="4"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="4"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="75">
@@ -1849,8 +1873,9 @@
     <hyperlink ref="A14" r:id="rId13"/>
     <hyperlink ref="A16" r:id="rId14"/>
     <hyperlink ref="A17" r:id="rId15"/>
+    <hyperlink ref="A18" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lvl has wall-jumping as well now
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -330,7 +330,8 @@
   <si>
     <t>Boost now only works if within range of a jump pad
 Rough Wall jump working
-modified level 7 a bit to force player to use wall jump in the beginning</t>
+modified level 7 a bit to force player to use wall jump in the beginning
+Level 8 wall jumping</t>
   </si>
 </sst>
 </file>
@@ -534,17 +535,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1244,43 +1245,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" spans="1:14" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
@@ -1501,14 +1502,14 @@
       <c r="A14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
@@ -1577,14 +1578,14 @@
       <c r="A18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
@@ -1611,7 +1612,7 @@
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
     </row>
-    <row r="20" spans="1:13" ht="45" customHeight="1">
+    <row r="20" spans="1:13" ht="58.5" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>82</v>
       </c>
@@ -1902,36 +1903,35 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1948,35 +1948,36 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
version 0.19 - better wall jump
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -332,6 +332,15 @@
 Rough Wall jump working
 modified level 7 a bit to force player to use wall jump in the beginning
 Level 8 wall jumping</t>
+  </si>
+  <si>
+    <t>v0.19</t>
+  </si>
+  <si>
+    <t>Changed wall jump to stop immediately when action button 1 is pressed
+Increased vertical velocity of wall jump, decreased horiztonal
+Cap for max/min jump pad velocities, still a small bug that sometimes stalls the character on the pad
+Rearranged levels slightly to accomodate for lower jumping height</t>
   </si>
 </sst>
 </file>
@@ -535,17 +544,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1235,7 +1244,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:G21"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1245,43 +1254,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
@@ -1502,14 +1511,14 @@
       <c r="A14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
@@ -1578,14 +1587,14 @@
       <c r="A18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
@@ -1631,9 +1640,13 @@
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
     </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="4"/>
-      <c r="B21" s="25"/>
+    <row r="21" spans="1:13" ht="72.75" customHeight="1">
+      <c r="A21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>85</v>
+      </c>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
@@ -1903,35 +1916,36 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1948,36 +1962,35 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -1998,8 +2011,9 @@
     <hyperlink ref="A18" r:id="rId16"/>
     <hyperlink ref="A19" r:id="rId17"/>
     <hyperlink ref="A20" r:id="rId18"/>
+    <hyperlink ref="A21" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 10th level, rough version
</commit_message>
<xml_diff>
--- a/see-saw-unity/Docs/todo.xlsx
+++ b/see-saw-unity/Docs/todo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15390" windowHeight="8565" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15390" windowHeight="8565"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>TODO LIST</t>
   </si>
@@ -351,6 +351,12 @@
   <si>
     <t>Hopefully fixed stall on jump pads
 Added level 9, rough version</t>
+  </si>
+  <si>
+    <t>v0.21</t>
+  </si>
+  <si>
+    <t>Added 10th level, rough version</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,9 +548,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -554,24 +557,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
@@ -633,27 +652,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B25" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B25" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
   <autoFilter ref="A2:B25"/>
   <sortState ref="A3:B25">
-    <sortCondition sortBy="cellColor" ref="A2:A25" dxfId="7"/>
+    <sortCondition sortBy="cellColor" ref="A2:A25" dxfId="1"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="2" name="Programming" dataDxfId="6"/>
-    <tableColumn id="8" name="Art" dataDxfId="5"/>
+    <tableColumn id="2" name="Programming" dataDxfId="8"/>
+    <tableColumn id="8" name="Art" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C2:C20" totalsRowShown="0" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C2:C20" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
   <autoFilter ref="C2:C20"/>
   <sortState ref="C3:C36">
-    <sortCondition sortBy="cellColor" ref="C2:C36" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="C2:C36" dxfId="3"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="Combined" dataDxfId="0"/>
+    <tableColumn id="1" name="Combined" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -946,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -959,11 +978,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
       <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5">
@@ -1028,9 +1047,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="30">
       <c r="A7" s="17" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1038,71 +1057,71 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="45">
       <c r="A8" s="16" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="17" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5">
       <c r="A11" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="16" t="s">
-        <v>77</v>
-      </c>
+      <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="22"/>
+      <c r="A13" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>75</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3" ht="45">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>78</v>
       </c>
       <c r="B17" s="17"/>
@@ -1255,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1266,701 +1285,706 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="1:14" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:14" ht="61.5" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
     </row>
     <row r="5" spans="1:14" ht="51.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:14" ht="127.5" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:14" ht="30.75" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:14" ht="33.75" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
     </row>
     <row r="10" spans="1:14" ht="45" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" spans="1:14" ht="112.5" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25" t="s">
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:14" ht="105.75" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:14" ht="58.5" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
     </row>
     <row r="14" spans="1:14" ht="16.5" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:14" ht="45.75" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:13" ht="120" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
     </row>
     <row r="19" spans="1:13" ht="59.25" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" ht="58.5" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" ht="72.75" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" ht="29.25" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="4"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
+      <c r="A23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="4"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="4"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="4"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="4"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="4"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="4"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="4"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="4"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="4"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="4"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="4"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="4"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B37:G37"/>
@@ -1977,36 +2001,35 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
@@ -2029,8 +2052,9 @@
     <hyperlink ref="A20" r:id="rId18"/>
     <hyperlink ref="A21" r:id="rId19"/>
     <hyperlink ref="A22" r:id="rId20"/>
+    <hyperlink ref="A23" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>